<commit_message>
post process pixel shaders
</commit_message>
<xml_diff>
--- a/Docs/Dev IV Project Rubric.xlsx
+++ b/Docs/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="I4" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="I8" s="18">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J8" s="18">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -2714,11 +2714,15 @@
       <c r="D75" s="5">
         <v>4</v>
       </c>
-      <c r="E75" s="2"/>
-      <c r="F75" s="3"/>
+      <c r="E75" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G75" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>

</xml_diff>

<commit_message>
optimized switch between cube and talon ship mesh
</commit_message>
<xml_diff>
--- a/Docs/Dev IV Project Rubric.xlsx
+++ b/Docs/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -374,6 +374,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -971,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1111,7 @@
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K4" s="18">
         <f>SUM(H6,I6,J6)</f>
@@ -1116,7 +1119,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1253,7 +1256,7 @@
       </c>
       <c r="J8" s="18">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1521,7 +1524,9 @@
       <c r="D20" s="5">
         <v>4</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="17">
         <f t="shared" si="0"/>
@@ -2979,7 +2984,9 @@
       <c r="D90" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E90" s="3"/>
+      <c r="E90" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
@@ -3001,7 +3008,9 @@
       <c r="D91" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
@@ -3134,7 +3143,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
render to texture triangle on cube
</commit_message>
<xml_diff>
--- a/Docs/Dev IV Project Rubric.xlsx
+++ b/Docs/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -975,7 +975,7 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K4" s="18">
         <f>SUM(H6,I6,J6)</f>
@@ -1119,7 +1119,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="J8" s="18">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1527,10 +1527,12 @@
       <c r="E20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G20" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -3143,7 +3145,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>